<commit_message>
buat menu perbarui npk
</commit_message>
<xml_diff>
--- a/assets/upload/format/form_kar_upload.xlsx
+++ b/assets/upload/format/form_kar_upload.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
   <si>
     <t>No.</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Permanent Employee</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
     <t>Junior Analyst</t>
   </si>
   <si>
@@ -159,15 +156,9 @@
     <t>Education Join</t>
   </si>
   <si>
-    <t>Education Update</t>
-  </si>
-  <si>
     <t>SMA</t>
   </si>
   <si>
-    <t>Karir</t>
-  </si>
-  <si>
     <t>Alamat KTP</t>
   </si>
   <si>
@@ -177,9 +168,6 @@
     <t>Kontak Darurat</t>
   </si>
   <si>
-    <t>Admin</t>
-  </si>
-  <si>
     <t>Priuk Jakarta Utara</t>
   </si>
   <si>
@@ -190,6 +178,84 @@
   </si>
   <si>
     <t>Join Date</t>
+  </si>
+  <si>
+    <t>Jurusan Pendidikan</t>
+  </si>
+  <si>
+    <t>Tahun Lulus</t>
+  </si>
+  <si>
+    <t>Nama Sekolah / Kampus</t>
+  </si>
+  <si>
+    <t>IPA</t>
+  </si>
+  <si>
+    <t>SMK DWIPA</t>
+  </si>
+  <si>
+    <t>Murry</t>
+  </si>
+  <si>
+    <t>Head Offie</t>
+  </si>
+  <si>
+    <t>Lodan Dalam II C RT 06 / RW 08 KEL.ANCOL JAKARTA UTARA</t>
+  </si>
+  <si>
+    <t>Bandung</t>
+  </si>
+  <si>
+    <t>0812-1212-2244</t>
+  </si>
+  <si>
+    <t>murrry@gmail.com</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>3175042312881111</t>
+  </si>
+  <si>
+    <t>3175042312881089</t>
+  </si>
+  <si>
+    <t>000124567892</t>
+  </si>
+  <si>
+    <t>120J12344</t>
+  </si>
+  <si>
+    <t>0001G31219801</t>
+  </si>
+  <si>
+    <t>246155097024001</t>
+  </si>
+  <si>
+    <t>6930347991</t>
+  </si>
+  <si>
+    <t>KAWIN</t>
+  </si>
+  <si>
+    <t>SMK</t>
+  </si>
+  <si>
+    <t>Operational</t>
+  </si>
+  <si>
+    <t>Ancol Jakarta Utara</t>
+  </si>
+  <si>
+    <t>0121212121</t>
+  </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMAN 1 </t>
   </si>
 </sst>
 </file>
@@ -197,7 +263,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -293,7 +359,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -315,7 +381,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="5" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -331,11 +397,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,10 +713,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AG3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,7 +732,7 @@
     <col min="9" max="9" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="5" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="19.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" style="5" bestFit="1" customWidth="1"/>
@@ -667,21 +746,22 @@
     <col min="24" max="24" width="14.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="20.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19" style="5" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="5"/>
+    <col min="27" max="27" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="18.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32">
+    <row r="1" spans="1:33">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
@@ -699,7 +779,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -753,28 +833,31 @@
         <v>22</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AA1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AD1" s="1" t="s">
-        <v>50</v>
+      <c r="AD1" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF1" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="15" customFormat="1">
+    <row r="2" spans="1:33" s="15" customFormat="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -782,7 +865,7 @@
         <v>123456</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>25</v>
@@ -797,7 +880,7 @@
         <v>28</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I2" s="9">
         <v>36251</v>
@@ -805,7 +888,7 @@
       <c r="J2" s="10">
         <v>51</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="L2" s="11" t="s">
@@ -851,25 +934,129 @@
         <v>41</v>
       </c>
       <c r="Z2" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AA2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AB2" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="AD2" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF2" s="19">
+      <c r="AB2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="18">
         <v>41955</v>
+      </c>
+      <c r="AE2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>2017</v>
+      </c>
+      <c r="AG2" s="19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33">
+      <c r="A3" s="23">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23">
+        <v>220220</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="9">
+        <v>35898</v>
+      </c>
+      <c r="J3" s="23">
+        <v>21</v>
+      </c>
+      <c r="K3" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="X3" s="13">
+        <v>123457</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AA3" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB3" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC3" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD3" s="18">
+        <v>40853</v>
+      </c>
+      <c r="AE3" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF3" s="23">
+        <v>2015</v>
+      </c>
+      <c r="AG3" s="24" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>